<commit_message>
Added a test for dates which isn't really complete.  I'd like to preparse things into dates from excel if we could know the data types before we parse.  The way we are parsing right now assumes everything is a string and is using a lot of classes from POI which makes these assumptions for us.  To do it another way and scale for really large sheets we'd have to modify those classes to create our own.
</commit_message>
<xml_diff>
--- a/src/test/resources/players.xlsx
+++ b/src/test/resources/players.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
   <si>
     <t>ID</t>
   </si>
@@ -78,12 +78,18 @@
   </si>
   <si>
     <t>score</t>
+  </si>
+  <si>
+    <t>birth_date</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="mm/dd/yy;@"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -113,8 +119,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -423,13 +430,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:F1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="12.85546875" style="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -445,8 +457,11 @@
       <c r="E1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -462,8 +477,11 @@
       <c r="E2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2" s="1">
+        <v>29305</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -479,8 +497,11 @@
       <c r="E3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3" s="1">
+        <v>27943</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -496,8 +517,11 @@
       <c r="E4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4" s="1">
+        <v>31272</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -513,8 +537,11 @@
       <c r="E5" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5" s="1">
+        <v>33134</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -530,8 +557,11 @@
       <c r="E6" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6" s="1">
+        <v>33647</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -547,8 +577,12 @@
       <c r="E7" t="s">
         <v>14</v>
       </c>
+      <c r="F7" s="1">
+        <v>28516</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fix gaps in excel sheets so we fill in the column properly when there are gaps in the rows.  Updated the test data to reflect a gappy spreadsheet.
</commit_message>
<xml_diff>
--- a/src/test/resources/players.xlsx
+++ b/src/test/resources/players.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
   <si>
     <t>ID</t>
   </si>
@@ -81,6 +81,12 @@
   </si>
   <si>
     <t>birth_date</t>
+  </si>
+  <si>
+    <t>Lim</t>
+  </si>
+  <si>
+    <t>Black</t>
   </si>
 </sst>
 </file>
@@ -88,7 +94,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="mm/dd/yy;@"/>
+    <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -121,7 +127,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -430,10 +436,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -581,6 +587,23 @@
         <v>28516</v>
       </c>
     </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" s="1">
+        <v>32511</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Fix date issues with Xlsx files where it'd return locale specific dates like 1/1/83 instead of 1/1/1983 or 1983-01-01.  Now it has a predictable default and you can override that default if you desire.
</commit_message>
<xml_diff>
--- a/src/test/resources/players.xlsx
+++ b/src/test/resources/players.xlsx
@@ -93,9 +93,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
-  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -127,7 +124,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -439,7 +436,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>